<commit_message>
corrected coordinates for Fort Lauderdale sampling site
Not worth re-running analyses, were only off by very little
</commit_message>
<xml_diff>
--- a/data_files/Master_Sample_List.xlsx
+++ b/data_files/Master_Sample_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erin_\Documents\Voss Lab (M.S.)\Lab Work\P.astreoides popgen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erin_\Documents\GitHub\SEFL_Pastreoides_2bRAD\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9FB98B-FA74-4A0E-895A-4358A077504C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16962AD1-04F7-4C56-A700-1D0267E3EBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="12" xr2:uid="{434D8A9B-0D0B-4ABF-AC04-A196659A4FA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{434D8A9B-0D0B-4ABF-AC04-A196659A4FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -2473,7 +2473,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2683,12 +2683,6 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -3540,7 +3534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="266">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4186,13 +4180,16 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4827,8 +4824,8 @@
   </sheetPr>
   <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5"/>
@@ -8683,11 +8680,11 @@
       <c r="G77" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H77" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I77" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H77" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I77" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J77" s="31">
         <v>32</v>
@@ -8733,11 +8730,11 @@
       <c r="G78" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H78" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I78" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H78" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I78" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J78" s="31">
         <v>33</v>
@@ -8783,11 +8780,11 @@
       <c r="G79" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H79" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I79" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H79" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I79" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J79" s="31">
         <v>34</v>
@@ -8833,11 +8830,11 @@
       <c r="G80" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H80" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I80" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H80" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I80" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J80" s="31">
         <v>35</v>
@@ -8883,11 +8880,11 @@
       <c r="G81" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H81" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I81" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H81" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I81" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J81" s="31">
         <v>327</v>
@@ -8933,11 +8930,11 @@
       <c r="G82" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H82" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I82" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H82" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I82" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J82" s="31">
         <v>328</v>
@@ -8983,11 +8980,11 @@
       <c r="G83" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H83" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I83" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H83" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I83" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J83" s="31">
         <v>329</v>
@@ -9033,11 +9030,11 @@
       <c r="G84" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H84" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I84" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H84" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I84" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J84" s="31">
         <v>330</v>
@@ -9083,11 +9080,11 @@
       <c r="G85" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H85" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I85" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H85" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I85" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J85" s="31">
         <v>341</v>
@@ -9133,11 +9130,11 @@
       <c r="G86" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H86" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I86" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H86" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I86" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J86" s="31">
         <v>342</v>
@@ -9183,11 +9180,11 @@
       <c r="G87" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H87" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I87" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H87" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I87" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J87" s="31">
         <v>343</v>
@@ -9233,11 +9230,11 @@
       <c r="G88" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H88" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I88" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H88" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I88" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J88" s="31">
         <v>344</v>
@@ -9283,11 +9280,11 @@
       <c r="G89" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H89" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I89" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H89" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I89" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J89" s="31">
         <v>345</v>
@@ -9333,11 +9330,11 @@
       <c r="G90" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H90" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I90" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H90" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I90" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J90" s="31">
         <v>346</v>
@@ -9383,11 +9380,11 @@
       <c r="G91" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H91" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I91" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H91" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I91" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J91" s="31">
         <v>347</v>
@@ -9633,11 +9630,11 @@
       <c r="G96" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H96" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I96" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H96" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I96" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J96" s="31">
         <v>33</v>
@@ -9683,11 +9680,11 @@
       <c r="G97" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H97" s="27">
-        <v>26.147866666666602</v>
-      </c>
-      <c r="I97" s="27">
-        <v>-80.093863333333303</v>
+      <c r="H97" s="265">
+        <v>26.147580000000001</v>
+      </c>
+      <c r="I97" s="265">
+        <v>-80.096100000000007</v>
       </c>
       <c r="J97" s="31">
         <v>33</v>
@@ -10524,7 +10521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E1FCEF-5961-4A04-8C69-6FACD2CEBA96}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -16545,8 +16542,8 @@
         <v>356</v>
       </c>
       <c r="U3" s="159"/>
-      <c r="V3" s="261"/>
-      <c r="W3" s="261"/>
+      <c r="V3" s="263"/>
+      <c r="W3" s="263"/>
     </row>
     <row r="4" spans="1:23" ht="16" thickBot="1">
       <c r="A4" s="124" t="s">
@@ -16604,8 +16601,8 @@
       <c r="U4" s="62" t="s">
         <v>358</v>
       </c>
-      <c r="V4" s="262"/>
-      <c r="W4" s="262"/>
+      <c r="V4" s="259"/>
+      <c r="W4" s="259"/>
     </row>
     <row r="5" spans="1:23" ht="16" thickBot="1">
       <c r="A5" s="124" t="s">
@@ -16663,8 +16660,8 @@
       <c r="U5" s="161" t="s">
         <v>359</v>
       </c>
-      <c r="V5" s="263"/>
-      <c r="W5" s="262"/>
+      <c r="V5" s="260"/>
+      <c r="W5" s="259"/>
     </row>
     <row r="6" spans="1:23" ht="16" thickBot="1">
       <c r="A6" s="124" t="s">
@@ -16783,8 +16780,8 @@
       <c r="U7" s="165" t="s">
         <v>361</v>
       </c>
-      <c r="V7" s="263"/>
-      <c r="W7" s="262"/>
+      <c r="V7" s="260"/>
+      <c r="W7" s="259"/>
     </row>
     <row r="8" spans="1:23" ht="16" thickBot="1">
       <c r="A8" s="124" t="s">
@@ -16835,11 +16832,11 @@
       <c r="Q8" s="147">
         <v>8.25</v>
       </c>
-      <c r="S8" s="259"/>
-      <c r="T8" s="260"/>
+      <c r="S8" s="261"/>
+      <c r="T8" s="262"/>
       <c r="U8" s="164"/>
-      <c r="V8" s="260"/>
-      <c r="W8" s="260"/>
+      <c r="V8" s="262"/>
+      <c r="W8" s="262"/>
     </row>
     <row r="9" spans="1:23" ht="16" thickBot="1">
       <c r="A9" s="124" t="s">
@@ -16866,11 +16863,11 @@
       <c r="Q9" s="150">
         <v>8.25</v>
       </c>
-      <c r="S9" s="261"/>
-      <c r="T9" s="261"/>
+      <c r="S9" s="263"/>
+      <c r="T9" s="263"/>
       <c r="U9" s="62"/>
-      <c r="V9" s="261"/>
-      <c r="W9" s="261"/>
+      <c r="V9" s="263"/>
+      <c r="W9" s="263"/>
     </row>
     <row r="10" spans="1:23" ht="16" thickBot="1">
       <c r="A10" s="126" t="s">
@@ -16903,11 +16900,11 @@
       <c r="Q10" s="153" t="s">
         <v>354</v>
       </c>
-      <c r="S10" s="262"/>
-      <c r="T10" s="262"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
       <c r="U10" s="62"/>
-      <c r="V10" s="262"/>
-      <c r="W10" s="262"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
     </row>
     <row r="11" spans="1:23" ht="16" thickBot="1">
       <c r="A11" s="132"/>
@@ -16939,8 +16936,8 @@
       <c r="U11" s="119">
         <v>75</v>
       </c>
-      <c r="V11" s="262"/>
-      <c r="W11" s="262"/>
+      <c r="V11" s="259"/>
+      <c r="W11" s="259"/>
     </row>
     <row r="12" spans="1:23" ht="16" customHeight="1">
       <c r="A12" t="s">
@@ -17057,8 +17054,8 @@
         <v>356</v>
       </c>
       <c r="U14" s="159"/>
-      <c r="V14" s="261"/>
-      <c r="W14" s="261"/>
+      <c r="V14" s="263"/>
+      <c r="W14" s="263"/>
     </row>
     <row r="15" spans="1:23" ht="16" thickBot="1">
       <c r="A15" s="124" t="s">
@@ -17116,8 +17113,8 @@
       <c r="U15" s="62" t="s">
         <v>358</v>
       </c>
-      <c r="V15" s="262"/>
-      <c r="W15" s="262"/>
+      <c r="V15" s="259"/>
+      <c r="W15" s="259"/>
     </row>
     <row r="16" spans="1:23" ht="16" thickBot="1">
       <c r="A16" s="124" t="s">
@@ -17175,8 +17172,8 @@
       <c r="U16" s="161" t="s">
         <v>359</v>
       </c>
-      <c r="V16" s="263"/>
-      <c r="W16" s="262"/>
+      <c r="V16" s="260"/>
+      <c r="W16" s="259"/>
     </row>
     <row r="17" spans="1:23" ht="16" thickBot="1">
       <c r="A17" s="124" t="s">
@@ -17295,8 +17292,8 @@
       <c r="U18" s="165" t="s">
         <v>361</v>
       </c>
-      <c r="V18" s="263"/>
-      <c r="W18" s="262"/>
+      <c r="V18" s="260"/>
+      <c r="W18" s="259"/>
     </row>
     <row r="19" spans="1:23" ht="16" thickBot="1">
       <c r="A19" s="124" t="s">
@@ -17347,11 +17344,11 @@
       <c r="Q19" s="147">
         <v>8.25</v>
       </c>
-      <c r="S19" s="259"/>
-      <c r="T19" s="260"/>
+      <c r="S19" s="261"/>
+      <c r="T19" s="262"/>
       <c r="U19" s="164"/>
-      <c r="V19" s="260"/>
-      <c r="W19" s="260"/>
+      <c r="V19" s="262"/>
+      <c r="W19" s="262"/>
     </row>
     <row r="20" spans="1:23" ht="16" thickBot="1">
       <c r="A20" s="126" t="s">
@@ -17378,11 +17375,11 @@
       <c r="Q20" s="150">
         <v>8.25</v>
       </c>
-      <c r="S20" s="261"/>
-      <c r="T20" s="261"/>
+      <c r="S20" s="263"/>
+      <c r="T20" s="263"/>
       <c r="U20" s="62"/>
-      <c r="V20" s="261"/>
-      <c r="W20" s="261"/>
+      <c r="V20" s="263"/>
+      <c r="W20" s="263"/>
     </row>
     <row r="21" spans="1:23" ht="16" thickBot="1">
       <c r="A21" s="136" t="s">
@@ -17415,11 +17412,11 @@
       <c r="Q21" s="153" t="s">
         <v>354</v>
       </c>
-      <c r="S21" s="262"/>
-      <c r="T21" s="262"/>
+      <c r="S21" s="259"/>
+      <c r="T21" s="259"/>
       <c r="U21" s="62"/>
-      <c r="V21" s="262"/>
-      <c r="W21" s="262"/>
+      <c r="V21" s="259"/>
+      <c r="W21" s="259"/>
     </row>
     <row r="22" spans="1:23" ht="16" thickBot="1">
       <c r="A22" s="130"/>
@@ -17451,8 +17448,8 @@
       <c r="U22" s="119">
         <v>75</v>
       </c>
-      <c r="V22" s="262"/>
-      <c r="W22" s="262"/>
+      <c r="V22" s="259"/>
+      <c r="W22" s="259"/>
     </row>
     <row r="23" spans="1:23" ht="16" thickBot="1">
       <c r="A23" s="138" t="s">
@@ -17519,8 +17516,8 @@
         <v>356</v>
       </c>
       <c r="U24" s="159"/>
-      <c r="V24" s="261"/>
-      <c r="W24" s="261"/>
+      <c r="V24" s="263"/>
+      <c r="W24" s="263"/>
     </row>
     <row r="25" spans="1:23" ht="16" thickBot="1">
       <c r="A25" s="128" t="s">
@@ -17578,8 +17575,8 @@
       <c r="U25" s="62" t="s">
         <v>358</v>
       </c>
-      <c r="V25" s="262"/>
-      <c r="W25" s="262"/>
+      <c r="V25" s="259"/>
+      <c r="W25" s="259"/>
     </row>
     <row r="26" spans="1:23" ht="16" thickBot="1">
       <c r="A26" s="124" t="s">
@@ -17637,8 +17634,8 @@
       <c r="U26" s="161" t="s">
         <v>359</v>
       </c>
-      <c r="V26" s="263"/>
-      <c r="W26" s="262"/>
+      <c r="V26" s="260"/>
+      <c r="W26" s="259"/>
     </row>
     <row r="27" spans="1:23" ht="16" thickBot="1">
       <c r="A27" s="124" t="s">
@@ -17757,8 +17754,8 @@
       <c r="U28" s="165" t="s">
         <v>361</v>
       </c>
-      <c r="V28" s="263"/>
-      <c r="W28" s="262"/>
+      <c r="V28" s="260"/>
+      <c r="W28" s="259"/>
     </row>
     <row r="29" spans="1:23" ht="16" thickBot="1">
       <c r="A29" s="124" t="s">
@@ -17801,11 +17798,11 @@
       <c r="Q29" s="147">
         <v>39.270000000000003</v>
       </c>
-      <c r="S29" s="259"/>
-      <c r="T29" s="260"/>
+      <c r="S29" s="261"/>
+      <c r="T29" s="262"/>
       <c r="U29" s="164"/>
-      <c r="V29" s="260"/>
-      <c r="W29" s="260"/>
+      <c r="V29" s="262"/>
+      <c r="W29" s="262"/>
     </row>
     <row r="30" spans="1:23" ht="16" thickBot="1">
       <c r="A30" s="124" t="s">
@@ -17832,11 +17829,11 @@
       <c r="Q30" s="147">
         <v>5.61</v>
       </c>
-      <c r="S30" s="261"/>
-      <c r="T30" s="261"/>
+      <c r="S30" s="263"/>
+      <c r="T30" s="263"/>
       <c r="U30" s="62"/>
-      <c r="V30" s="261"/>
-      <c r="W30" s="261"/>
+      <c r="V30" s="263"/>
+      <c r="W30" s="263"/>
     </row>
     <row r="31" spans="1:23" ht="16" thickBot="1">
       <c r="A31" s="124" t="s">
@@ -17863,11 +17860,11 @@
       <c r="Q31" s="150">
         <v>5.61</v>
       </c>
-      <c r="S31" s="262"/>
-      <c r="T31" s="262"/>
+      <c r="S31" s="259"/>
+      <c r="T31" s="259"/>
       <c r="U31" s="62"/>
-      <c r="V31" s="262"/>
-      <c r="W31" s="262"/>
+      <c r="V31" s="259"/>
+      <c r="W31" s="259"/>
     </row>
     <row r="32" spans="1:23" ht="16" thickBot="1">
       <c r="A32" s="124" t="s">
@@ -17907,8 +17904,8 @@
       <c r="U32" s="119">
         <v>51</v>
       </c>
-      <c r="V32" s="262"/>
-      <c r="W32" s="262"/>
+      <c r="V32" s="259"/>
+      <c r="W32" s="259"/>
     </row>
     <row r="33" spans="15:17" ht="16" thickBot="1">
       <c r="O33" s="154" t="s">
@@ -17923,14 +17920,18 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="V11:W11"/>
     <mergeCell ref="V26:W26"/>
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
@@ -17944,18 +17945,14 @@
     <mergeCell ref="V22:W22"/>
     <mergeCell ref="V24:W24"/>
     <mergeCell ref="V25:W25"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="V31:W31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20925,8 +20922,8 @@
       <c r="Q10" s="62"/>
     </row>
     <row r="11" spans="1:19" ht="16" thickBot="1">
-      <c r="A11" s="262"/>
-      <c r="B11" s="262"/>
+      <c r="A11" s="259"/>
+      <c r="B11" s="259"/>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
       <c r="E11" s="62"/>
@@ -21032,8 +21029,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5">
-      <c r="A14" s="262"/>
-      <c r="B14" s="262"/>
+      <c r="A14" s="259"/>
+      <c r="B14" s="259"/>
       <c r="C14" s="62"/>
       <c r="D14" s="62"/>
       <c r="E14" s="62"/>
@@ -21057,8 +21054,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.5">
-      <c r="A15" s="262"/>
-      <c r="B15" s="262"/>
+      <c r="A15" s="259"/>
+      <c r="B15" s="259"/>
       <c r="C15" s="62"/>
       <c r="D15" s="62"/>
       <c r="E15" s="62"/>
@@ -21082,8 +21079,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.5">
-      <c r="A16" s="262"/>
-      <c r="B16" s="262"/>
+      <c r="A16" s="259"/>
+      <c r="B16" s="259"/>
       <c r="C16" s="62"/>
       <c r="D16" s="62"/>
       <c r="E16" s="62"/>
@@ -21107,8 +21104,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.5">
-      <c r="A17" s="262"/>
-      <c r="B17" s="262"/>
+      <c r="A17" s="259"/>
+      <c r="B17" s="259"/>
       <c r="C17" s="62"/>
       <c r="D17" s="62"/>
       <c r="E17" s="62"/>
@@ -21132,8 +21129,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="15.5">
-      <c r="A18" s="262"/>
-      <c r="B18" s="262"/>
+      <c r="A18" s="259"/>
+      <c r="B18" s="259"/>
       <c r="C18" s="62"/>
       <c r="D18" s="62"/>
       <c r="E18" s="62"/>
@@ -21157,8 +21154,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="16" thickBot="1">
-      <c r="A19" s="262"/>
-      <c r="B19" s="262"/>
+      <c r="A19" s="259"/>
+      <c r="B19" s="259"/>
       <c r="C19" s="62"/>
       <c r="D19" s="62"/>
       <c r="E19" s="62"/>
@@ -21182,8 +21179,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" ht="16" thickBot="1">
-      <c r="A20" s="262"/>
-      <c r="B20" s="262"/>
+      <c r="A20" s="259"/>
+      <c r="B20" s="259"/>
       <c r="C20" s="62"/>
       <c r="D20" s="62"/>
       <c r="E20" s="62"/>
@@ -21207,8 +21204,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.5">
-      <c r="A21" s="262"/>
-      <c r="B21" s="262"/>
+      <c r="A21" s="259"/>
+      <c r="B21" s="259"/>
       <c r="C21" s="62"/>
       <c r="D21" s="62"/>
       <c r="E21" s="62"/>
@@ -21226,8 +21223,8 @@
       <c r="Q21" s="62"/>
     </row>
     <row r="22" spans="1:17" ht="42">
-      <c r="A22" s="262"/>
-      <c r="B22" s="262"/>
+      <c r="A22" s="259"/>
+      <c r="B22" s="259"/>
       <c r="C22" s="62"/>
       <c r="D22" s="62"/>
       <c r="E22" s="62"/>
@@ -21249,8 +21246,8 @@
       <c r="Q22" s="62"/>
     </row>
     <row r="23" spans="1:17" ht="28">
-      <c r="A23" s="262"/>
-      <c r="B23" s="262"/>
+      <c r="A23" s="259"/>
+      <c r="B23" s="259"/>
       <c r="C23" s="62"/>
       <c r="D23" s="62"/>
       <c r="E23" s="62"/>
@@ -21274,8 +21271,8 @@
       <c r="Q23" s="62"/>
     </row>
     <row r="24" spans="1:17" ht="15.5">
-      <c r="A24" s="262"/>
-      <c r="B24" s="262"/>
+      <c r="A24" s="259"/>
+      <c r="B24" s="259"/>
       <c r="C24" s="62"/>
       <c r="D24" s="62"/>
       <c r="E24" s="62"/>
@@ -21294,12 +21291,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
     <mergeCell ref="J23:N23"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A14:B14"/>
@@ -21307,6 +21298,12 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>